<commit_message>
get back newAssignment from the fetch
</commit_message>
<xml_diff>
--- a/algorithm/requirements.xlsx
+++ b/algorithm/requirements.xlsx
@@ -432,16 +432,16 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
       <c r="E1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -455,16 +455,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -483,11 +483,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -501,16 +501,16 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -570,16 +570,16 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -593,16 +593,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -616,16 +616,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -639,16 +639,16 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -662,12 +662,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -685,16 +685,16 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -708,16 +708,16 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -731,16 +731,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -754,16 +754,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -777,16 +777,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -800,16 +800,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -823,16 +823,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -846,16 +846,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -869,16 +869,16 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -892,12 +892,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -915,16 +915,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -938,16 +938,16 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -961,16 +961,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -993,7 +993,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -1007,16 +1007,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1030,16 +1030,16 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1053,16 +1053,16 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -1076,16 +1076,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1099,16 +1099,16 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1145,16 +1145,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -1168,12 +1168,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1191,16 +1191,16 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1214,12 +1214,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1237,16 +1237,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1260,16 +1260,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1283,16 +1283,16 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">
@@ -1306,16 +1306,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1352,16 +1352,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -1375,16 +1375,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -1421,16 +1421,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -1444,16 +1444,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
@@ -1467,16 +1467,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -1490,16 +1490,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48">
@@ -1513,16 +1513,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
@@ -1536,16 +1536,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -1559,12 +1559,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1582,16 +1582,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52">
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
@@ -1628,16 +1628,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -1651,16 +1651,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1683,7 +1683,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -1697,16 +1697,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
@@ -1720,16 +1720,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58">
@@ -1743,16 +1743,16 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
@@ -1766,16 +1766,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -1789,16 +1789,16 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -1812,16 +1812,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1844,7 +1844,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63">
@@ -1858,16 +1858,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
@@ -1904,16 +1904,16 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
@@ -1927,16 +1927,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -1950,12 +1950,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -1973,16 +1973,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69">
@@ -1996,16 +1996,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2042,16 +2042,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72">
@@ -2065,16 +2065,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
@@ -2088,16 +2088,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -2111,16 +2111,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
@@ -2134,12 +2134,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
           <t>08:00</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>09:00</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2157,16 +2157,16 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -2180,16 +2180,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -2203,16 +2203,16 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79">
@@ -2226,16 +2226,16 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
@@ -2249,16 +2249,16 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -2272,16 +2272,16 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
@@ -2300,11 +2300,11 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
@@ -2318,16 +2318,16 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84">
@@ -2341,16 +2341,16 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -2364,16 +2364,16 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
@@ -2387,16 +2387,16 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -2410,16 +2410,16 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -2433,16 +2433,16 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89">
@@ -2456,16 +2456,16 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90">
@@ -2479,16 +2479,16 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91">
@@ -2502,16 +2502,16 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92">
@@ -2525,16 +2525,16 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
@@ -2548,16 +2548,16 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94">
@@ -2571,16 +2571,16 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95">
@@ -2594,16 +2594,16 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96">
@@ -2617,16 +2617,16 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97">
@@ -2640,16 +2640,16 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98">
@@ -2668,11 +2668,11 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2709,16 +2709,16 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101">
@@ -2732,16 +2732,16 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102">
@@ -2755,16 +2755,16 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
@@ -2778,16 +2778,16 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
@@ -2801,16 +2801,16 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -2824,16 +2824,16 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106">
@@ -2847,16 +2847,16 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107">
@@ -2870,16 +2870,16 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108">
@@ -2893,16 +2893,16 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109">
@@ -2916,16 +2916,16 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
@@ -2939,16 +2939,16 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
@@ -2962,16 +2962,16 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112">
@@ -2985,16 +2985,16 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113">
@@ -3008,12 +3008,12 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -3031,16 +3031,16 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
@@ -3054,16 +3054,16 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -3077,16 +3077,16 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
@@ -3100,16 +3100,16 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118">
@@ -3123,16 +3123,16 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119">
@@ -3146,16 +3146,16 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120">
@@ -3169,12 +3169,12 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -3215,12 +3215,12 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -3238,16 +3238,16 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3284,16 +3284,16 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126">
@@ -3307,16 +3307,16 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E126" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127">
@@ -3330,16 +3330,16 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
@@ -3353,16 +3353,16 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
@@ -3376,12 +3376,12 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -3399,16 +3399,16 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131">
@@ -3422,16 +3422,16 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E131" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132">
@@ -3445,16 +3445,16 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133">
@@ -3468,16 +3468,16 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134">
@@ -3491,16 +3491,16 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135">
@@ -3514,16 +3514,16 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
@@ -3537,12 +3537,12 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -3560,16 +3560,16 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
@@ -3606,16 +3606,16 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -3652,16 +3652,16 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E141" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
@@ -3675,16 +3675,16 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143">
@@ -3698,16 +3698,16 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144">
@@ -3721,16 +3721,16 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145">
@@ -3744,16 +3744,16 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>11:00</t>
-        </is>
-      </c>
       <c r="E145" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146">
@@ -3767,16 +3767,16 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -3790,16 +3790,16 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148">
@@ -3813,16 +3813,16 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="149">
@@ -3836,16 +3836,16 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E149" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150">
@@ -3859,16 +3859,16 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E150" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151">
@@ -3882,16 +3882,16 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E151" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152">
@@ -3905,16 +3905,16 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153">
@@ -3928,16 +3928,16 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154">
@@ -3951,16 +3951,16 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E154" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155">
@@ -3974,16 +3974,16 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E155" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156">
@@ -3997,16 +3997,16 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157">
@@ -4020,12 +4020,12 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -4043,16 +4043,16 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159">
@@ -4066,12 +4066,12 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -4089,16 +4089,16 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E160" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161">
@@ -4112,16 +4112,16 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162">
@@ -4135,16 +4135,16 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E162" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="163">
@@ -4158,16 +4158,16 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E163" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164">
@@ -4181,16 +4181,16 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
       <c r="E164" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="165">
@@ -4204,16 +4204,16 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E165" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="166">
@@ -4227,16 +4227,16 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E166" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167">
@@ -4250,16 +4250,16 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168">
@@ -4273,16 +4273,16 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -4296,16 +4296,16 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E169" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="170">
@@ -4319,16 +4319,16 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E170" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
@@ -4342,7 +4342,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -4351,7 +4351,7 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172">
@@ -4365,12 +4365,12 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -4388,12 +4388,12 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -4411,16 +4411,16 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E174" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -4443,7 +4443,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -4457,16 +4457,16 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E176" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -4480,16 +4480,16 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E177" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178">
@@ -4503,16 +4503,16 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E178" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179">
@@ -4526,16 +4526,16 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E179" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180">
@@ -4549,12 +4549,12 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
           <t>10:00</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>11:00</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -4572,16 +4572,16 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E181" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182">
@@ -4595,16 +4595,16 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E182" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183">
@@ -4618,16 +4618,16 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E183" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184">
@@ -4641,16 +4641,16 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E184" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185">
@@ -4664,16 +4664,16 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E185" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
@@ -4687,12 +4687,12 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -4710,16 +4710,16 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E187" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188">
@@ -4733,16 +4733,16 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E188" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189">
@@ -4756,16 +4756,16 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E189" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190">
@@ -4779,16 +4779,16 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E190" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="191">
@@ -4811,7 +4811,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
@@ -4825,16 +4825,16 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E192" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -4848,16 +4848,16 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E193" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194">
@@ -4871,16 +4871,16 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E194" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195">
@@ -4894,16 +4894,16 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D195" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E195" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="196">
@@ -4917,16 +4917,16 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E196" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197">
@@ -4940,16 +4940,16 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E197" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198">
@@ -4968,11 +4968,11 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E198" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="199">
@@ -4986,12 +4986,12 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -5009,16 +5009,16 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E200" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201">
@@ -5037,11 +5037,11 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E201" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
@@ -5055,16 +5055,16 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E202" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203">
@@ -5083,11 +5083,11 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E203" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204">
@@ -5101,12 +5101,12 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -5124,16 +5124,16 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E205" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206">
@@ -5147,16 +5147,16 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E206" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207">
@@ -5170,16 +5170,16 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E207" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="208">
@@ -5198,11 +5198,11 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E208" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="209">
@@ -5216,16 +5216,16 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E209" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210">
@@ -5239,16 +5239,16 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E210" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211">
@@ -5262,12 +5262,12 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -5285,16 +5285,16 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E212" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213">
@@ -5308,16 +5308,16 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E213" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="214">
@@ -5331,16 +5331,16 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E214" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="215">
@@ -5354,16 +5354,16 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E215" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216">
@@ -5377,12 +5377,12 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E216" t="n">
@@ -5400,16 +5400,16 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E217" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -5446,16 +5446,16 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E219" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220">
@@ -5474,11 +5474,11 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E220" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="221">
@@ -5492,12 +5492,12 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -5515,16 +5515,16 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E222" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="223">
@@ -5538,16 +5538,16 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E223" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224">
@@ -5561,16 +5561,16 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E224" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="225">
@@ -5584,16 +5584,16 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E225" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="226">
@@ -5607,16 +5607,16 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E226" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227">
@@ -5630,16 +5630,16 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E227" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="228">
@@ -5653,16 +5653,16 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E228" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229">
@@ -5676,12 +5676,12 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E229" t="n">
@@ -5699,16 +5699,16 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E230" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="231">
@@ -5722,16 +5722,16 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E231" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="232">
@@ -5768,16 +5768,16 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E233" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="234">
@@ -5791,16 +5791,16 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E234" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235">
@@ -5814,16 +5814,16 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E235" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="236">
@@ -5837,16 +5837,16 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E236" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="237">
@@ -5860,16 +5860,16 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E237" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="238">
@@ -5883,16 +5883,16 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E238" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239">
@@ -5906,16 +5906,16 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E239" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="240">
@@ -5929,16 +5929,16 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D240" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E240" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
newAssignment return from server
</commit_message>
<xml_diff>
--- a/algorithm/requirements.xlsx
+++ b/algorithm/requirements.xlsx
@@ -432,16 +432,16 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -455,16 +455,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -501,16 +501,16 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -570,16 +570,16 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -593,16 +593,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -616,16 +616,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -639,16 +639,16 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -662,16 +662,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -685,16 +685,16 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -708,7 +708,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -731,12 +731,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>11:00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>15:00</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -754,16 +754,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -777,7 +777,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -800,16 +800,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -823,16 +823,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -846,16 +846,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -869,16 +869,16 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -892,16 +892,16 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -915,12 +915,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -938,7 +938,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -961,16 +961,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -984,12 +984,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1007,16 +1007,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1030,16 +1030,16 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
@@ -1053,16 +1053,16 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1076,16 +1076,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1108,7 +1108,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -1122,16 +1122,16 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1145,12 +1145,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1168,16 +1168,16 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -1191,16 +1191,16 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
@@ -1214,16 +1214,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -1237,16 +1237,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -1260,16 +1260,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
@@ -1283,12 +1283,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1306,16 +1306,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -1329,12 +1329,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1357,11 +1357,11 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -1375,16 +1375,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -1398,16 +1398,16 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -1490,16 +1490,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -1513,16 +1513,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -1536,16 +1536,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -1568,7 +1568,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -1582,12 +1582,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1605,16 +1605,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -1628,16 +1628,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -1651,16 +1651,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
@@ -1674,16 +1674,16 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
@@ -1697,16 +1697,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -1720,16 +1720,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
@@ -1748,11 +1748,11 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -1766,16 +1766,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -1789,16 +1789,16 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -1812,16 +1812,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -1835,16 +1835,16 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -1858,16 +1858,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64">
@@ -1886,11 +1886,11 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -1927,16 +1927,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -1950,16 +1950,16 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -1973,16 +1973,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -1996,16 +1996,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70">
@@ -2019,16 +2019,16 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71">
@@ -2042,16 +2042,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
@@ -2065,16 +2065,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -2093,11 +2093,11 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -2134,12 +2134,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2157,16 +2157,16 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -2180,16 +2180,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -2203,16 +2203,16 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
@@ -2226,16 +2226,16 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80">
@@ -2249,16 +2249,16 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -2272,16 +2272,16 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -2295,16 +2295,16 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -2318,16 +2318,16 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -2341,16 +2341,16 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2373,7 +2373,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86">
@@ -2387,16 +2387,16 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -2410,16 +2410,16 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
@@ -2433,16 +2433,16 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89">
@@ -2456,16 +2456,16 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
@@ -2479,16 +2479,16 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -2502,16 +2502,16 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
@@ -2525,16 +2525,16 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
@@ -2548,16 +2548,16 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -2571,12 +2571,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -2594,16 +2594,16 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
@@ -2617,16 +2617,16 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -2663,12 +2663,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -2686,16 +2686,16 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100">
@@ -2709,12 +2709,12 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -2732,12 +2732,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -2755,16 +2755,16 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103">
@@ -2778,16 +2778,16 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
           <t>17:00</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>21:00</t>
-        </is>
-      </c>
       <c r="E103" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104">
@@ -2801,16 +2801,16 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105">
@@ -2824,16 +2824,16 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106">
@@ -2847,7 +2847,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2856,7 +2856,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107">
@@ -2870,16 +2870,16 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
@@ -2893,12 +2893,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -2962,16 +2962,16 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
@@ -2985,16 +2985,16 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113">
@@ -3008,16 +3008,16 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115">
@@ -3054,16 +3054,16 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116">
@@ -3077,16 +3077,16 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117">
@@ -3100,16 +3100,16 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
       <c r="E117" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
@@ -3123,16 +3123,16 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
@@ -3146,16 +3146,16 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
@@ -3169,16 +3169,16 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121">
@@ -3192,16 +3192,16 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122">
@@ -3215,16 +3215,16 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123">
@@ -3238,16 +3238,16 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124">
@@ -3261,16 +3261,16 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
@@ -3284,16 +3284,16 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126">
@@ -3307,16 +3307,16 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127">
@@ -3330,16 +3330,16 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128">
@@ -3353,16 +3353,16 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129">
@@ -3376,16 +3376,16 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130">
@@ -3399,16 +3399,16 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131">
@@ -3422,16 +3422,16 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
       <c r="E131" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -3445,12 +3445,12 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -3491,16 +3491,16 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135">
@@ -3514,16 +3514,16 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -3537,12 +3537,12 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -3560,12 +3560,12 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -3583,16 +3583,16 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139">
@@ -3606,16 +3606,16 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E139" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140">
@@ -3629,16 +3629,16 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="141">
@@ -3652,12 +3652,12 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -3675,16 +3675,16 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
@@ -3698,12 +3698,12 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -3721,16 +3721,16 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145">
@@ -3744,16 +3744,16 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E145" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146">
@@ -3767,16 +3767,16 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -3813,12 +3813,12 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E148" t="n">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3845,7 +3845,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150">
@@ -3859,16 +3859,16 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E150" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151">
@@ -3882,12 +3882,12 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -3905,16 +3905,16 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153">
@@ -3928,16 +3928,16 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154">
@@ -3951,16 +3951,16 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E154" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155">
@@ -3974,16 +3974,16 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156">
@@ -3997,16 +3997,16 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="157">
@@ -4020,16 +4020,16 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E157" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158">
@@ -4043,16 +4043,16 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="159">
@@ -4066,16 +4066,16 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E159" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160">
@@ -4089,12 +4089,12 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -4112,16 +4112,16 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162">
@@ -4135,16 +4135,16 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E162" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="163">
@@ -4158,12 +4158,12 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E163" t="n">
@@ -4181,16 +4181,16 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E164" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -4204,16 +4204,16 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E165" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -4250,16 +4250,16 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="168">
@@ -4273,16 +4273,16 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E168" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169">
@@ -4296,16 +4296,16 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
       <c r="E169" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170">
@@ -4319,12 +4319,12 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -4342,16 +4342,16 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E171" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172">
@@ -4374,7 +4374,7 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -4397,7 +4397,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174">
@@ -4411,16 +4411,16 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E174" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175">
@@ -4443,7 +4443,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176">
@@ -4457,16 +4457,16 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E176" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177">
@@ -4480,16 +4480,16 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
           <t>17:00</t>
         </is>
       </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
       <c r="E177" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178">
@@ -4503,16 +4503,16 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E178" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179">
@@ -4526,16 +4526,16 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E179" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -4549,12 +4549,12 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -4572,12 +4572,12 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -4604,7 +4604,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183">
@@ -4618,16 +4618,16 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E183" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184">
@@ -4641,16 +4641,16 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E184" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185">
@@ -4664,16 +4664,16 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E185" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="186">
@@ -4687,16 +4687,16 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E186" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187">
@@ -4719,7 +4719,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188">
@@ -4733,16 +4733,16 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E188" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="189">
@@ -4756,16 +4756,16 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E189" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="190">
@@ -4779,16 +4779,16 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E190" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
@@ -4802,16 +4802,16 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E191" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="192">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -4848,16 +4848,16 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E193" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="194">
@@ -4871,16 +4871,16 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E194" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195">
@@ -4894,16 +4894,16 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E195" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196">
@@ -4917,16 +4917,16 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E196" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197">
@@ -4940,16 +4940,16 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E197" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198">
@@ -4963,16 +4963,16 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E198" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="199">
@@ -4986,16 +4986,16 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E199" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200">
@@ -5009,16 +5009,16 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E200" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="201">
@@ -5032,16 +5032,16 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E201" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="202">
@@ -5055,16 +5055,16 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E202" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="203">
@@ -5078,16 +5078,16 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E203" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204">
@@ -5101,16 +5101,16 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E204" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205">
@@ -5124,16 +5124,16 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E205" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="206">
@@ -5147,12 +5147,12 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -5170,16 +5170,16 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E207" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208">
@@ -5193,16 +5193,16 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E208" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="209">
@@ -5221,11 +5221,11 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E209" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="210">
@@ -5239,16 +5239,16 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E210" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211">
@@ -5262,16 +5262,16 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E211" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="212">
@@ -5285,16 +5285,16 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E212" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="213">
@@ -5308,16 +5308,16 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E213" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="214">
@@ -5331,16 +5331,16 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E214" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="215">
@@ -5354,16 +5354,16 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E215" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
@@ -5377,16 +5377,16 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E216" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217">
@@ -5400,16 +5400,16 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E217" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="218">
@@ -5423,16 +5423,16 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E218" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="219">
@@ -5446,12 +5446,12 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -5469,16 +5469,16 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E220" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="221">
@@ -5492,16 +5492,16 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E221" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="222">
@@ -5515,16 +5515,16 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E222" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="223">
@@ -5538,16 +5538,16 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E223" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="224">
@@ -5561,16 +5561,16 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E224" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="225">
@@ -5584,16 +5584,16 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E225" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="226">
@@ -5607,16 +5607,16 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E226" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227">
@@ -5630,16 +5630,16 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E227" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228">
@@ -5653,12 +5653,12 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E228" t="n">
@@ -5676,16 +5676,16 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E229" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="230">
@@ -5699,16 +5699,16 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E230" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231">
@@ -5722,16 +5722,16 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E231" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="232">
@@ -5745,16 +5745,16 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D232" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E232" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233">
@@ -5768,16 +5768,16 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E233" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234">
@@ -5791,16 +5791,16 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E234" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
@@ -5814,16 +5814,16 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E235" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236">
@@ -5837,16 +5837,16 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E236" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="237">
@@ -5860,16 +5860,16 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E237" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="238">
@@ -5892,7 +5892,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="239">
@@ -5906,16 +5906,16 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E239" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
           <t>09:00</t>
-        </is>
-      </c>
-      <c r="D240" t="inlineStr">
-        <is>
-          <t>13:00</t>
         </is>
       </c>
       <c r="E240" t="n">

</xml_diff>

<commit_message>
page table shows assignment
</commit_message>
<xml_diff>
--- a/algorithm/requirements.xlsx
+++ b/algorithm/requirements.xlsx
@@ -432,16 +432,16 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -455,16 +455,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -501,16 +501,16 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -570,16 +570,16 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -593,16 +593,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -616,16 +616,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -639,7 +639,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -662,16 +662,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -708,16 +708,16 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -731,16 +731,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -754,16 +754,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -777,16 +777,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -800,16 +800,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -823,16 +823,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -846,16 +846,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -869,16 +869,16 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -892,16 +892,16 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -915,16 +915,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -947,7 +947,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -961,16 +961,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>12:00</t>
-        </is>
-      </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -984,16 +984,16 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -1007,16 +1007,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1030,16 +1030,16 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -1058,11 +1058,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
@@ -1076,16 +1076,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1099,16 +1099,16 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1122,16 +1122,16 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1145,16 +1145,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
@@ -1168,16 +1168,16 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -1191,12 +1191,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1214,16 +1214,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -1237,16 +1237,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1260,16 +1260,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1283,16 +1283,16 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1306,16 +1306,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1329,12 +1329,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1352,12 +1352,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1375,16 +1375,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1398,12 +1398,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1421,16 +1421,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
@@ -1444,16 +1444,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
@@ -1467,16 +1467,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -1490,16 +1490,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -1513,16 +1513,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
@@ -1536,12 +1536,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1559,16 +1559,16 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
@@ -1582,16 +1582,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1605,16 +1605,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
@@ -1628,16 +1628,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -1651,16 +1651,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -1679,11 +1679,11 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
@@ -1702,11 +1702,11 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -1743,16 +1743,16 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -1766,16 +1766,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
@@ -1789,16 +1789,16 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61">
@@ -1812,16 +1812,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -1835,16 +1835,16 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -1858,16 +1858,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64">
@@ -1881,16 +1881,16 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
@@ -1904,12 +1904,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -1927,16 +1927,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -1950,16 +1950,16 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
@@ -1973,16 +1973,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
@@ -1996,12 +1996,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2019,16 +2019,16 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -2042,12 +2042,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2065,16 +2065,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
@@ -2088,16 +2088,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -2111,16 +2111,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -2134,16 +2134,16 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
@@ -2157,16 +2157,16 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -2180,16 +2180,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
@@ -2226,12 +2226,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2249,16 +2249,16 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
@@ -2272,16 +2272,16 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
@@ -2295,16 +2295,16 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
@@ -2318,16 +2318,16 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
@@ -2341,12 +2341,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2364,16 +2364,16 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -2387,16 +2387,16 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -2415,11 +2415,11 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
@@ -2433,16 +2433,16 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89">
@@ -2456,16 +2456,16 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90">
@@ -2479,16 +2479,16 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91">
@@ -2507,11 +2507,11 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
@@ -2525,16 +2525,16 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -2548,16 +2548,16 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94">
@@ -2571,16 +2571,16 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
@@ -2594,16 +2594,16 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
@@ -2617,16 +2617,16 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
@@ -2640,16 +2640,16 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98">
@@ -2663,12 +2663,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -2686,12 +2686,12 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -2709,16 +2709,16 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101">
@@ -2732,16 +2732,16 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102">
@@ -2755,16 +2755,16 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103">
@@ -2778,12 +2778,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -2810,7 +2810,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -2824,16 +2824,16 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106">
@@ -2847,16 +2847,16 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107">
@@ -2870,16 +2870,16 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108">
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
@@ -2916,16 +2916,16 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
@@ -2939,16 +2939,16 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111">
@@ -2962,16 +2962,16 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
@@ -2985,16 +2985,16 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113">
@@ -3036,11 +3036,11 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -3077,16 +3077,16 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
           <t>08:00</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
       <c r="E116" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
@@ -3100,16 +3100,16 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
@@ -3123,16 +3123,16 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119">
@@ -3146,16 +3146,16 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120">
@@ -3169,16 +3169,16 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E120" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121">
@@ -3192,16 +3192,16 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E121" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122">
@@ -3215,16 +3215,16 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="E122" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123">
@@ -3238,16 +3238,16 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
@@ -3266,11 +3266,11 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125">
@@ -3284,16 +3284,16 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
@@ -3307,16 +3307,16 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127">
@@ -3335,11 +3335,11 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128">
@@ -3353,16 +3353,16 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
@@ -3376,16 +3376,16 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130">
@@ -3399,16 +3399,16 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E130" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131">
@@ -3422,16 +3422,16 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132">
@@ -3445,16 +3445,16 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133">
@@ -3468,12 +3468,12 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -3491,16 +3491,16 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
@@ -3514,16 +3514,16 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137">
@@ -3560,16 +3560,16 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138">
@@ -3583,16 +3583,16 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139">
@@ -3606,12 +3606,12 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -3652,16 +3652,16 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E141" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142">
@@ -3675,16 +3675,16 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143">
@@ -3698,16 +3698,16 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144">
@@ -3721,16 +3721,16 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145">
@@ -3744,16 +3744,16 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E145" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146">
@@ -3767,16 +3767,16 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147">
@@ -3790,16 +3790,16 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149">
@@ -3836,16 +3836,16 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E149" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150">
@@ -3859,16 +3859,16 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="E150" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151">
@@ -3882,16 +3882,16 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
       <c r="E151" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152">
@@ -3905,16 +3905,16 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153">
@@ -3928,16 +3928,16 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154">
@@ -3951,16 +3951,16 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E154" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155">
@@ -3974,16 +3974,16 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -3997,16 +3997,16 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157">
@@ -4020,16 +4020,16 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E157" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158">
@@ -4043,16 +4043,16 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E158" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159">
@@ -4066,16 +4066,16 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
       <c r="E159" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160">
@@ -4089,16 +4089,16 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E160" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -4112,16 +4112,16 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E161" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162">
@@ -4135,16 +4135,16 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E162" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163">
@@ -4158,16 +4158,16 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E163" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164">
@@ -4181,16 +4181,16 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E164" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165">
@@ -4204,16 +4204,16 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>20:00</t>
-        </is>
-      </c>
       <c r="E165" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="166">
@@ -4227,16 +4227,16 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E166" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167">
@@ -4250,16 +4250,16 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E167" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -4296,16 +4296,16 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E169" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170">
@@ -4319,16 +4319,16 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>14:00</t>
-        </is>
-      </c>
       <c r="E170" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="171">
@@ -4342,16 +4342,16 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E171" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="172">
@@ -4365,16 +4365,16 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E172" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173">
@@ -4388,16 +4388,16 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E173" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174">
@@ -4411,16 +4411,16 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E174" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="175">
@@ -4434,16 +4434,16 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E175" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -4457,16 +4457,16 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E176" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177">
@@ -4480,16 +4480,16 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E177" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178">
@@ -4508,11 +4508,11 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E178" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179">
@@ -4526,16 +4526,16 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E179" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180">
@@ -4549,16 +4549,16 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E180" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181">
@@ -4572,16 +4572,16 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E181" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182">
@@ -4595,12 +4595,12 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
           <t>12:00</t>
-        </is>
-      </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>13:00</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -4618,12 +4618,12 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -4646,11 +4646,11 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E184" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185">
@@ -4664,16 +4664,16 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E185" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186">
@@ -4687,16 +4687,16 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E186" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187">
@@ -4710,16 +4710,16 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E187" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188">
@@ -4733,12 +4733,12 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -4756,16 +4756,16 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>21:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E189" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -4779,12 +4779,12 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -4802,16 +4802,16 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E191" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
@@ -4825,16 +4825,16 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E192" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193">
@@ -4848,16 +4848,16 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E193" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194">
@@ -4871,16 +4871,16 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E194" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195">
@@ -4894,7 +4894,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -4903,7 +4903,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -4917,16 +4917,16 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E196" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197">
@@ -4940,16 +4940,16 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E197" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="198">
@@ -4963,16 +4963,16 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E198" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="199">
@@ -4986,16 +4986,16 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E199" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200">
@@ -5009,16 +5009,16 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E200" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201">
@@ -5032,16 +5032,16 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E201" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202">
@@ -5055,16 +5055,16 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="D202" t="inlineStr">
-        <is>
-          <t>10:00</t>
-        </is>
-      </c>
       <c r="E202" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203">
@@ -5078,16 +5078,16 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E203" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="204">
@@ -5101,16 +5101,16 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E204" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="205">
@@ -5124,16 +5124,16 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E205" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206">
@@ -5147,16 +5147,16 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="D206" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E206" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207">
@@ -5170,12 +5170,12 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -5193,16 +5193,16 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E208" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209">
@@ -5216,12 +5216,12 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -5239,16 +5239,16 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E210" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="211">
@@ -5262,16 +5262,16 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E211" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212">
@@ -5285,16 +5285,16 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E212" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213">
@@ -5313,11 +5313,11 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E213" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="214">
@@ -5331,16 +5331,16 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E214" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="215">
@@ -5354,16 +5354,16 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E215" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="216">
@@ -5377,16 +5377,16 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E216" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217">
@@ -5400,16 +5400,16 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E217" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218">
@@ -5423,16 +5423,16 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E218" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="219">
@@ -5446,16 +5446,16 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E219" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="220">
@@ -5469,16 +5469,16 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D220" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
       <c r="E220" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221">
@@ -5492,16 +5492,16 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="E221" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222">
@@ -5515,16 +5515,16 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E222" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223">
@@ -5538,16 +5538,16 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E223" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="224">
@@ -5561,12 +5561,12 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -5584,16 +5584,16 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E225" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="226">
@@ -5607,16 +5607,16 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E226" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227">
@@ -5630,16 +5630,16 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E227" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="228">
@@ -5653,16 +5653,16 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E228" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="229">
@@ -5676,16 +5676,16 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D229" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E229" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230">
@@ -5708,7 +5708,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="231">
@@ -5722,16 +5722,16 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E231" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="232">
@@ -5745,16 +5745,16 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E232" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="233">
@@ -5768,12 +5768,12 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E233" t="n">
@@ -5796,11 +5796,11 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E234" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="235">
@@ -5819,11 +5819,11 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E235" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="236">
@@ -5837,16 +5837,16 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="E236" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="237">
@@ -5860,12 +5860,12 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E237" t="n">
@@ -5883,16 +5883,16 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D238" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
       <c r="E238" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239">
@@ -5906,16 +5906,16 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E239" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="240">
@@ -5929,12 +5929,12 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E240" t="n">

</xml_diff>